<commit_message>
Mapping TwoHeadersPivotTable to PivotTable
</commit_message>
<xml_diff>
--- a/tests/ExcelProcesser.Tests/resources/real world samples/19SPX16合同生产细节.xlsx
+++ b/tests/ExcelProcesser.Tests/resources/real world samples/19SPX16合同生产细节.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22829"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24117"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VsCode\Github\ExcelProcesser\tests\ExcelProcesser.Tests\resources\real world samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5B6278C-EEB7-4458-A53D-C37110D280F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8CBEA4-FBB5-400C-AFD4-C483036CB6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macro1" sheetId="4" state="hidden" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$B$1:$P$186</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,6 +34,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -281,6 +303,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>印配码</t>
@@ -335,6 +358,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>规格：</t>
@@ -351,6 +375,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>务必扫描得出来！！！）</t>
@@ -492,8 +517,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="40">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -762,6 +787,12 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1985,8 +2016,8 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3049,44 +3080,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:A7"/>
   <sheetViews>
     <sheetView showFormulas="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="e">
         <f>#N/A</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="e">
         <f>#N/A</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="e">
         <f>#N/A</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -3100,14 +3131,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P351"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.3984375" customWidth="1"/>
     <col min="2" max="2" width="15.69921875" customWidth="1"/>
@@ -3118,7 +3149,7 @@
     <col min="10" max="10" width="18.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="36" customHeight="1">
+    <row r="1" spans="2:15" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="92" t="s">
         <v>0</v>
       </c>
@@ -3133,7 +3164,7 @@
       <c r="K1" s="92"/>
       <c r="L1" s="92"/>
     </row>
-    <row r="2" spans="2:15" ht="21.9" customHeight="1">
+    <row r="2" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="93" t="s">
@@ -3147,7 +3178,7 @@
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="2:15" ht="21.9" customHeight="1">
+    <row r="3" spans="2:15" ht="21.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3161,7 +3192,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="2:15" ht="20.399999999999999">
+    <row r="4" spans="2:15" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -3169,17 +3200,17 @@
       <c r="N4" s="18"/>
       <c r="O4" s="19"/>
     </row>
-    <row r="5" spans="2:15" ht="13.5" customHeight="1">
+    <row r="5" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
@@ -3190,8 +3221,21 @@
         <v>8</v>
       </c>
       <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="L7">
+        <v>3000</v>
+      </c>
+      <c r="M7" cm="1">
+        <f t="array" ref="M7:O19">_xll.IdSaveTransfer(L7:L9,6,8)</f>
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>1000</v>
+      </c>
+      <c r="O7" t="str">
+        <v>1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 2 2 2 2 2 2 2 2 2 2 2 2 2 2 2 2 2 2 3 3 3 3 3 3 3 3 3 3 3 3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
@@ -3202,8 +3246,20 @@
         <v>10</v>
       </c>
       <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="2:15">
+      <c r="L8">
+        <v>3000</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>1000</v>
+      </c>
+      <c r="O8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
@@ -3213,24 +3269,63 @@
       <c r="F9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="2:15">
+      <c r="L9">
+        <v>3000</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>1500</v>
+      </c>
+      <c r="O9" t="str">
+        <v>共买1040元</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="2:15">
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="str">
+        <v>共卖900元</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="str">
+        <v xml:space="preserve"> 至少印550张</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="2:15">
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
@@ -3241,8 +3336,17 @@
         <v>8</v>
       </c>
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="2:15">
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
@@ -3253,8 +3357,17 @@
         <v>10</v>
       </c>
       <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="2:15">
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
@@ -3265,24 +3378,60 @@
         <v>16</v>
       </c>
       <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="2:15">
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="2:7">
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="2:7">
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="2:7">
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>18</v>
       </c>
@@ -3293,8 +3442,17 @@
         <v>19</v>
       </c>
       <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="2:7">
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
@@ -3306,7 +3464,7 @@
       </c>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>6</v>
       </c>
@@ -3318,7 +3476,7 @@
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>11</v>
       </c>
@@ -3330,23 +3488,23 @@
       </c>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>18</v>
       </c>
@@ -3358,7 +3516,7 @@
       </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>15</v>
       </c>
@@ -3370,7 +3528,7 @@
       </c>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>24</v>
       </c>
@@ -3382,15 +3540,15 @@
       </c>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="32" spans="2:7">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>26</v>
       </c>
@@ -3400,7 +3558,7 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
         <v>27</v>
       </c>
@@ -3411,21 +3569,21 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" spans="2:14">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="2:14">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
@@ -3436,7 +3594,7 @@
       </c>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" spans="2:14">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="12" t="s">
@@ -3448,7 +3606,7 @@
       </c>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="2:14">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="12"/>
       <c r="C38" s="13"/>
       <c r="D38" s="12" t="s">
@@ -3463,7 +3621,7 @@
       <c r="K38" s="11"/>
       <c r="L38" s="11"/>
     </row>
-    <row r="39" spans="2:14">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -3476,7 +3634,7 @@
       <c r="M39" s="11"/>
       <c r="N39" s="11"/>
     </row>
-    <row r="40" spans="2:14">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -3486,7 +3644,7 @@
       </c>
       <c r="G40" s="16"/>
     </row>
-    <row r="41" spans="2:14">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -3496,26 +3654,26 @@
       </c>
       <c r="G41" s="16"/>
     </row>
-    <row r="42" spans="2:14">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D42" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="10"/>
     </row>
-    <row r="44" spans="2:14">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="2:14">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="2:14">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -3523,7 +3681,7 @@
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="2:14">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="9" t="s">
         <v>37</v>
       </c>
@@ -3538,7 +3696,7 @@
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
     </row>
-    <row r="48" spans="2:14">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
         <v>38</v>
       </c>
@@ -3553,7 +3711,7 @@
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
     </row>
-    <row r="49" spans="2:16">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
@@ -3567,7 +3725,7 @@
       <c r="L49" s="9"/>
       <c r="P49" s="20"/>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>39</v>
       </c>
@@ -3583,7 +3741,7 @@
       <c r="L50" s="9"/>
       <c r="P50" s="21"/>
     </row>
-    <row r="51" spans="2:16" ht="17.399999999999999">
+    <row r="51" spans="2:16" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>40</v>
       </c>
@@ -3599,7 +3757,7 @@
       <c r="L51" s="9"/>
       <c r="P51" s="22"/>
     </row>
-    <row r="52" spans="2:16" ht="17.399999999999999">
+    <row r="52" spans="2:16" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>41</v>
       </c>
@@ -3615,7 +3773,7 @@
       <c r="L52" s="9"/>
       <c r="P52" s="22"/>
     </row>
-    <row r="53" spans="2:16">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
@@ -3628,7 +3786,7 @@
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="2:16">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
@@ -3641,7 +3799,7 @@
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
     </row>
-    <row r="55" spans="2:16">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
@@ -3654,7 +3812,7 @@
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
     </row>
-    <row r="56" spans="2:16">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -3667,7 +3825,7 @@
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="2:16" ht="20.100000000000001" customHeight="1">
+    <row r="57" spans="2:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -3680,7 +3838,7 @@
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
     </row>
-    <row r="58" spans="2:16" ht="12.75" customHeight="1">
+    <row r="58" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -3693,7 +3851,7 @@
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
     </row>
-    <row r="59" spans="2:16">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
@@ -3706,7 +3864,7 @@
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
     </row>
-    <row r="60" spans="2:16">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
@@ -3719,7 +3877,7 @@
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
     </row>
-    <row r="61" spans="2:16">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
@@ -3733,7 +3891,7 @@
       <c r="L61" s="9"/>
       <c r="M61" s="23"/>
     </row>
-    <row r="62" spans="2:16" ht="18" customHeight="1">
+    <row r="62" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
@@ -3749,7 +3907,7 @@
       <c r="L62" s="9"/>
       <c r="M62" s="23"/>
     </row>
-    <row r="63" spans="2:16" ht="15" customHeight="1">
+    <row r="63" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
@@ -3765,7 +3923,7 @@
       <c r="L63" s="9"/>
       <c r="M63" s="23"/>
     </row>
-    <row r="64" spans="2:16" ht="14.25" customHeight="1">
+    <row r="64" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
@@ -3779,7 +3937,7 @@
       <c r="L64" s="9"/>
       <c r="M64" s="23"/>
     </row>
-    <row r="65" spans="2:14" ht="15" customHeight="1">
+    <row r="65" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
@@ -3793,7 +3951,7 @@
       <c r="L65" s="9"/>
       <c r="M65" s="23"/>
     </row>
-    <row r="66" spans="2:14" ht="15" customHeight="1">
+    <row r="66" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
@@ -3807,7 +3965,7 @@
       <c r="L66" s="9"/>
       <c r="M66" s="23"/>
     </row>
-    <row r="67" spans="2:14">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
@@ -3821,7 +3979,7 @@
       <c r="L67" s="9"/>
       <c r="M67" s="23"/>
     </row>
-    <row r="68" spans="2:14">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
@@ -3835,7 +3993,7 @@
       <c r="L68" s="9"/>
       <c r="M68" s="23"/>
     </row>
-    <row r="69" spans="2:14" ht="18" customHeight="1">
+    <row r="69" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
@@ -3849,7 +4007,7 @@
       <c r="L69" s="9"/>
       <c r="M69" s="23"/>
     </row>
-    <row r="70" spans="2:14" ht="15.75" customHeight="1">
+    <row r="70" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
@@ -3863,7 +4021,7 @@
       <c r="L70" s="9"/>
       <c r="M70" s="23"/>
     </row>
-    <row r="71" spans="2:14" ht="14.25" customHeight="1">
+    <row r="71" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
@@ -3877,7 +4035,7 @@
       <c r="L71" s="9"/>
       <c r="M71" s="23"/>
     </row>
-    <row r="72" spans="2:14" ht="15" customHeight="1">
+    <row r="72" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
@@ -3891,7 +4049,7 @@
       <c r="L72" s="9"/>
       <c r="M72" s="23"/>
     </row>
-    <row r="73" spans="2:14" ht="12.75" customHeight="1">
+    <row r="73" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="s">
         <v>44</v>
       </c>
@@ -3907,7 +4065,7 @@
       <c r="L73" s="9"/>
       <c r="M73" s="23"/>
     </row>
-    <row r="74" spans="2:14" ht="12.75" customHeight="1">
+    <row r="74" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="9" t="s">
         <v>45</v>
       </c>
@@ -3923,7 +4081,7 @@
       <c r="L74" s="9"/>
       <c r="M74" s="23"/>
     </row>
-    <row r="75" spans="2:14">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
         <v>46</v>
       </c>
@@ -3938,7 +4096,7 @@
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
     </row>
-    <row r="76" spans="2:14">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
@@ -3951,7 +4109,7 @@
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
     </row>
-    <row r="77" spans="2:14">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
@@ -3964,7 +4122,7 @@
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
     </row>
-    <row r="78" spans="2:14">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
@@ -3977,7 +4135,7 @@
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
     </row>
-    <row r="79" spans="2:14" ht="17.399999999999999">
+    <row r="79" spans="2:14" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
@@ -3992,7 +4150,7 @@
       <c r="M79" s="22"/>
       <c r="N79" s="22"/>
     </row>
-    <row r="80" spans="2:14" ht="17.399999999999999">
+    <row r="80" spans="2:14" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
@@ -4007,7 +4165,7 @@
       <c r="M80" s="22"/>
       <c r="N80" s="22"/>
     </row>
-    <row r="81" spans="2:14" ht="17.399999999999999">
+    <row r="81" spans="2:14" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
@@ -4022,7 +4180,7 @@
       <c r="M81" s="22"/>
       <c r="N81" s="22"/>
     </row>
-    <row r="82" spans="2:14">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
@@ -4035,7 +4193,7 @@
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
     </row>
-    <row r="83" spans="2:14">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
@@ -4050,7 +4208,7 @@
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
     </row>
-    <row r="84" spans="2:14">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
@@ -4063,7 +4221,7 @@
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
     </row>
-    <row r="85" spans="2:14">
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
@@ -4076,7 +4234,7 @@
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
     </row>
-    <row r="86" spans="2:14">
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
@@ -4089,7 +4247,7 @@
       <c r="K86" s="9"/>
       <c r="L86" s="9"/>
     </row>
-    <row r="87" spans="2:14" ht="17.399999999999999">
+    <row r="87" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B87" s="24" t="s">
         <v>48</v>
       </c>
@@ -4104,7 +4262,7 @@
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
     </row>
-    <row r="88" spans="2:14">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B88" s="25" t="s">
         <v>49</v>
       </c>
@@ -4119,7 +4277,7 @@
       <c r="K88" s="9"/>
       <c r="L88" s="9"/>
     </row>
-    <row r="89" spans="2:14">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
@@ -4132,7 +4290,7 @@
       <c r="K89" s="9"/>
       <c r="L89" s="9"/>
     </row>
-    <row r="90" spans="2:14">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B90" s="7" t="s">
         <v>50</v>
       </c>
@@ -4147,7 +4305,7 @@
       <c r="K90" s="9"/>
       <c r="L90" s="9"/>
     </row>
-    <row r="91" spans="2:14">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B91" s="9" t="s">
         <v>51</v>
       </c>
@@ -4162,7 +4320,7 @@
       <c r="K91" s="9"/>
       <c r="L91" s="9"/>
     </row>
-    <row r="92" spans="2:14">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B92" s="9" t="s">
         <v>52</v>
       </c>
@@ -4177,7 +4335,7 @@
       <c r="K92" s="9"/>
       <c r="L92" s="9"/>
     </row>
-    <row r="93" spans="2:14">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
@@ -4190,7 +4348,7 @@
       <c r="K93" s="9"/>
       <c r="L93" s="9"/>
     </row>
-    <row r="94" spans="2:14">
+    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B94" s="26"/>
       <c r="C94" s="27"/>
       <c r="D94" s="27"/>
@@ -4209,7 +4367,7 @@
       <c r="K94" s="9"/>
       <c r="L94" s="9"/>
     </row>
-    <row r="95" spans="2:14">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B95" s="31"/>
       <c r="C95" s="32"/>
       <c r="D95" s="33"/>
@@ -4228,7 +4386,7 @@
       <c r="K95" s="9"/>
       <c r="L95" s="9"/>
     </row>
-    <row r="96" spans="2:14">
+    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B96" s="31"/>
       <c r="C96" s="32"/>
       <c r="D96" s="32"/>
@@ -4247,7 +4405,7 @@
       <c r="K96" s="9"/>
       <c r="L96" s="9"/>
     </row>
-    <row r="97" spans="1:14" ht="84.9" customHeight="1">
+    <row r="97" spans="1:14" ht="84.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="31"/>
       <c r="C97" s="32"/>
       <c r="D97" s="32"/>
@@ -4262,7 +4420,7 @@
       <c r="K97" s="9"/>
       <c r="L97" s="9"/>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B98" s="39" t="s">
         <v>53</v>
       </c>
@@ -4283,7 +4441,7 @@
       <c r="K98" s="9"/>
       <c r="L98" s="9"/>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B99" s="39" t="s">
         <v>65</v>
       </c>
@@ -4306,7 +4464,7 @@
       <c r="K99" s="9"/>
       <c r="L99" s="9"/>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B100" s="39" t="s">
         <v>70</v>
       </c>
@@ -4327,7 +4485,7 @@
       <c r="K100" s="9"/>
       <c r="L100" s="9"/>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B101" s="44"/>
       <c r="C101" s="45" t="s">
         <v>73</v>
@@ -4346,7 +4504,7 @@
       <c r="K101" s="9"/>
       <c r="L101" s="9"/>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
       <c r="D102" s="9"/>
@@ -4359,7 +4517,7 @@
       <c r="K102" s="9"/>
       <c r="L102" s="9"/>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
@@ -4372,7 +4530,7 @@
       <c r="K103" s="9"/>
       <c r="L103" s="9"/>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B104" s="7" t="s">
         <v>76</v>
       </c>
@@ -4387,7 +4545,7 @@
       <c r="K104" s="9"/>
       <c r="L104" s="9"/>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B105" s="25" t="s">
         <v>77</v>
       </c>
@@ -4404,7 +4562,7 @@
       <c r="M105" s="16"/>
       <c r="N105" s="16"/>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B106" s="25" t="s">
         <v>78</v>
       </c>
@@ -4421,7 +4579,7 @@
       <c r="M106" s="16"/>
       <c r="N106" s="16"/>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
       <c r="D107" s="9"/>
@@ -4434,7 +4592,7 @@
       <c r="K107" s="9"/>
       <c r="L107" s="9"/>
     </row>
-    <row r="108" spans="1:14">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="11"/>
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
@@ -4448,7 +4606,7 @@
       <c r="K108" s="9"/>
       <c r="L108" s="9"/>
     </row>
-    <row r="109" spans="1:14">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="11"/>
       <c r="B109" s="9" t="s">
         <v>79</v>
@@ -4464,7 +4622,7 @@
       <c r="K109" s="9"/>
       <c r="L109" s="9"/>
     </row>
-    <row r="110" spans="1:14">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="11"/>
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
@@ -4478,7 +4636,7 @@
       <c r="K110" s="9"/>
       <c r="L110" s="9"/>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="11"/>
       <c r="B111" s="11" t="s">
         <v>80</v>
@@ -4494,7 +4652,7 @@
       <c r="K111" s="9"/>
       <c r="L111" s="9"/>
     </row>
-    <row r="112" spans="1:14">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="11"/>
       <c r="B112" s="11" t="s">
         <v>81</v>
@@ -4510,7 +4668,7 @@
       <c r="K112" s="9"/>
       <c r="L112" s="9"/>
     </row>
-    <row r="113" spans="1:14" ht="18.75" customHeight="1">
+    <row r="113" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="11"/>
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
@@ -4524,7 +4682,7 @@
       <c r="K113" s="9"/>
       <c r="L113" s="9"/>
     </row>
-    <row r="114" spans="1:14" ht="18.75" customHeight="1">
+    <row r="114" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="11"/>
       <c r="B114" s="50" t="s">
         <v>82</v>
@@ -4540,7 +4698,7 @@
       <c r="K114" s="9"/>
       <c r="L114" s="9"/>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="11"/>
       <c r="B115" s="51" t="s">
         <v>83</v>
@@ -4548,7 +4706,7 @@
       <c r="K115" s="9"/>
       <c r="L115" s="9"/>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="11"/>
       <c r="B116" s="51" t="s">
         <v>84</v>
@@ -4556,7 +4714,7 @@
       <c r="K116" s="9"/>
       <c r="L116" s="9"/>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="11"/>
       <c r="B117" s="51" t="s">
         <v>85</v>
@@ -4564,7 +4722,7 @@
       <c r="K117" s="9"/>
       <c r="L117" s="9"/>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="11"/>
       <c r="B118" s="51" t="s">
         <v>86</v>
@@ -4572,7 +4730,7 @@
       <c r="K118" s="9"/>
       <c r="L118" s="9"/>
     </row>
-    <row r="119" spans="1:14">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="11"/>
       <c r="B119" s="52" t="s">
         <v>87</v>
@@ -4584,30 +4742,30 @@
       <c r="K119" s="9"/>
       <c r="L119" s="9"/>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B120" s="51"/>
       <c r="F120" s="51"/>
       <c r="K120" s="9"/>
       <c r="L120" s="9"/>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B121" s="51"/>
       <c r="F121" s="51"/>
       <c r="K121" s="9"/>
       <c r="L121" s="9"/>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B122" s="6"/>
       <c r="L122" s="9"/>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B123" s="54"/>
       <c r="E123" s="6"/>
       <c r="G123" s="54"/>
       <c r="L123" s="9"/>
       <c r="N123" s="6"/>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B124" s="54"/>
       <c r="E124" s="6"/>
       <c r="G124" s="54"/>
@@ -4615,28 +4773,28 @@
       <c r="L124" s="9"/>
       <c r="N124" s="6"/>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
       <c r="E125" s="6"/>
       <c r="J125" s="51"/>
       <c r="L125" s="9"/>
       <c r="N125" s="6"/>
     </row>
-    <row r="126" spans="1:14" ht="17.399999999999999">
+    <row r="126" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B126" s="55"/>
       <c r="E126" s="6"/>
       <c r="G126" s="16"/>
       <c r="L126" s="9"/>
       <c r="M126" s="22"/>
     </row>
-    <row r="127" spans="1:14" ht="17.399999999999999">
+    <row r="127" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="E127" s="6"/>
       <c r="J127" s="8"/>
       <c r="K127" s="64"/>
       <c r="L127" s="9"/>
       <c r="M127" s="22"/>
     </row>
-    <row r="128" spans="1:14" ht="17.399999999999999">
+    <row r="128" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
       <c r="E128" s="6"/>
@@ -4647,7 +4805,7 @@
       <c r="L128" s="9"/>
       <c r="M128" s="22"/>
     </row>
-    <row r="129" spans="1:13" ht="15" customHeight="1">
+    <row r="129" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="55"/>
       <c r="E129" s="6"/>
       <c r="I129" s="82"/>
@@ -4656,7 +4814,7 @@
       <c r="L129" s="11"/>
       <c r="M129" s="22"/>
     </row>
-    <row r="130" spans="1:13" ht="17.399999999999999">
+    <row r="130" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="E130" s="6"/>
       <c r="F130" s="51"/>
       <c r="G130" s="65"/>
@@ -4668,7 +4826,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="17.399999999999999">
+    <row r="131" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A131" s="11"/>
       <c r="C131" s="66"/>
       <c r="D131" s="66"/>
@@ -4682,7 +4840,7 @@
       <c r="L131" s="11"/>
       <c r="M131" s="22"/>
     </row>
-    <row r="132" spans="1:13" ht="17.399999999999999">
+    <row r="132" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A132" s="11"/>
       <c r="B132" s="67" t="s">
         <v>90</v>
@@ -4701,7 +4859,7 @@
       <c r="L132" s="22"/>
       <c r="M132" s="22"/>
     </row>
-    <row r="133" spans="1:13" ht="17.399999999999999">
+    <row r="133" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A133" s="11"/>
       <c r="B133" s="69" t="s">
         <v>92</v>
@@ -4720,7 +4878,7 @@
       <c r="L133" s="22"/>
       <c r="M133" s="22"/>
     </row>
-    <row r="134" spans="1:13" ht="17.399999999999999">
+    <row r="134" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A134" s="11"/>
       <c r="B134" s="69" t="s">
         <v>94</v>
@@ -4739,7 +4897,7 @@
       <c r="L134" s="22"/>
       <c r="M134" s="22"/>
     </row>
-    <row r="135" spans="1:13" ht="21" customHeight="1">
+    <row r="135" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="71" t="s">
         <v>96</v>
       </c>
@@ -4753,7 +4911,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="19.95" customHeight="1">
+    <row r="136" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B136" s="67" t="s">
         <v>98</v>
       </c>
@@ -4770,7 +4928,7 @@
       <c r="K136" s="94"/>
       <c r="L136" s="94"/>
     </row>
-    <row r="137" spans="1:13" ht="33" customHeight="1">
+    <row r="137" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B137" t="s">
         <v>100</v>
       </c>
@@ -4784,7 +4942,7 @@
       <c r="K137" s="95"/>
       <c r="L137" s="95"/>
     </row>
-    <row r="138" spans="1:13" ht="25.8">
+    <row r="138" spans="1:13" ht="25.8" x14ac:dyDescent="0.4">
       <c r="B138" t="s">
         <v>102</v>
       </c>
@@ -4798,7 +4956,7 @@
       <c r="K138" s="96"/>
       <c r="L138" s="96"/>
     </row>
-    <row r="139" spans="1:13" ht="34.950000000000003" customHeight="1">
+    <row r="139" spans="1:13" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B139" t="s">
         <v>104</v>
       </c>
@@ -4812,7 +4970,7 @@
       <c r="K139" s="95"/>
       <c r="L139" s="95"/>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B140" s="11"/>
       <c r="C140" s="11"/>
       <c r="D140" s="11"/>
@@ -4826,7 +4984,7 @@
       <c r="L140" s="11"/>
       <c r="M140" s="11"/>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B141" s="11"/>
       <c r="C141" s="11"/>
       <c r="D141" s="11"/>
@@ -4840,7 +4998,7 @@
       <c r="L141" s="11"/>
       <c r="M141" s="11"/>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B142" s="11"/>
       <c r="C142" s="11"/>
       <c r="D142" s="11"/>
@@ -4854,7 +5012,7 @@
       <c r="L142" s="11"/>
       <c r="M142" s="11"/>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B143" s="11"/>
       <c r="C143" s="11"/>
       <c r="D143" s="11"/>
@@ -4867,30 +5025,30 @@
       <c r="L143" s="11"/>
       <c r="M143" s="11"/>
     </row>
-    <row r="144" spans="1:13" ht="21" customHeight="1">
+    <row r="144" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B144" s="51"/>
       <c r="G144" s="74"/>
       <c r="H144" s="74"/>
       <c r="I144" s="84"/>
       <c r="M144" s="11"/>
     </row>
-    <row r="146" spans="2:13" ht="25.8">
+    <row r="146" spans="2:13" ht="25.8" x14ac:dyDescent="0.4">
       <c r="B146" s="76"/>
       <c r="G146" s="74"/>
       <c r="H146" s="74"/>
       <c r="I146" s="84"/>
     </row>
-    <row r="147" spans="2:13" ht="25.8">
+    <row r="147" spans="2:13" ht="25.8" x14ac:dyDescent="0.4">
       <c r="G147" s="74"/>
       <c r="H147" s="74"/>
       <c r="I147" s="84"/>
     </row>
-    <row r="148" spans="2:13" ht="25.8">
+    <row r="148" spans="2:13" ht="25.8" x14ac:dyDescent="0.4">
       <c r="G148" s="74"/>
       <c r="H148" s="74"/>
       <c r="I148" s="84"/>
     </row>
-    <row r="149" spans="2:13" ht="25.8">
+    <row r="149" spans="2:13" ht="25.8" x14ac:dyDescent="0.4">
       <c r="F149" t="s">
         <v>89</v>
       </c>
@@ -4898,7 +5056,7 @@
       <c r="H149" s="74"/>
       <c r="I149" s="84"/>
     </row>
-    <row r="150" spans="2:13" ht="25.8">
+    <row r="150" spans="2:13" ht="25.8" x14ac:dyDescent="0.4">
       <c r="B150" s="69" t="s">
         <v>106</v>
       </c>
@@ -4906,7 +5064,7 @@
       <c r="H150" s="74"/>
       <c r="I150" s="84"/>
     </row>
-    <row r="151" spans="2:13" ht="20.100000000000001" customHeight="1">
+    <row r="151" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B151" s="77" t="s">
         <v>107</v>
       </c>
@@ -4918,7 +5076,7 @@
       <c r="H151" s="74"/>
       <c r="I151" s="84"/>
     </row>
-    <row r="152" spans="2:13" ht="13.95" customHeight="1">
+    <row r="152" spans="2:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B152" t="s">
         <v>97</v>
       </c>
@@ -4926,7 +5084,7 @@
       <c r="H152" s="74"/>
       <c r="I152" s="84"/>
     </row>
-    <row r="153" spans="2:13" ht="13.95" customHeight="1">
+    <row r="153" spans="2:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B153" t="s">
         <v>108</v>
       </c>
@@ -4935,7 +5093,7 @@
       <c r="H153" s="74"/>
       <c r="I153" s="84"/>
     </row>
-    <row r="154" spans="2:13" ht="15" customHeight="1">
+    <row r="154" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B154" t="s">
         <v>109</v>
       </c>
@@ -4944,7 +5102,7 @@
       <c r="H154" s="74"/>
       <c r="I154" s="84"/>
     </row>
-    <row r="155" spans="2:13" ht="25.8">
+    <row r="155" spans="2:13" ht="25.8" x14ac:dyDescent="0.4">
       <c r="B155" t="s">
         <v>110</v>
       </c>
@@ -4953,7 +5111,7 @@
       <c r="H155" s="74"/>
       <c r="I155" s="84"/>
     </row>
-    <row r="156" spans="2:13">
+    <row r="156" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B156" s="11" t="s">
         <v>104</v>
       </c>
@@ -4969,7 +5127,7 @@
       <c r="L156" s="11"/>
       <c r="M156" s="11"/>
     </row>
-    <row r="157" spans="2:13" ht="16.5" customHeight="1">
+    <row r="157" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="11"/>
       <c r="C157" s="11"/>
       <c r="D157" s="11"/>
@@ -4983,7 +5141,7 @@
       <c r="L157" s="11"/>
       <c r="M157" s="11"/>
     </row>
-    <row r="158" spans="2:13" ht="18" customHeight="1">
+    <row r="158" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="11"/>
       <c r="C158" s="11"/>
       <c r="D158" s="11"/>
@@ -4997,7 +5155,7 @@
       <c r="L158" s="11"/>
       <c r="M158" s="11"/>
     </row>
-    <row r="159" spans="2:13" ht="21" customHeight="1">
+    <row r="159" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="11"/>
       <c r="C159" s="11"/>
       <c r="D159" s="11"/>
@@ -5011,7 +5169,7 @@
       <c r="L159" s="11"/>
       <c r="M159" s="11"/>
     </row>
-    <row r="160" spans="2:13">
+    <row r="160" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
       <c r="D160" s="9"/>
@@ -5025,7 +5183,7 @@
       <c r="L160" s="9"/>
       <c r="M160" s="11"/>
     </row>
-    <row r="161" spans="2:13">
+    <row r="161" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
       <c r="D161" s="9"/>
@@ -5039,7 +5197,7 @@
       <c r="L161" s="9"/>
       <c r="M161" s="11"/>
     </row>
-    <row r="162" spans="2:13">
+    <row r="162" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
       <c r="D162" s="9"/>
@@ -5053,7 +5211,7 @@
       <c r="L162" s="9"/>
       <c r="M162" s="11"/>
     </row>
-    <row r="163" spans="2:13">
+    <row r="163" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
       <c r="D163" s="9"/>
@@ -5067,7 +5225,7 @@
       <c r="L163" s="9"/>
       <c r="M163" s="11"/>
     </row>
-    <row r="164" spans="2:13">
+    <row r="164" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
       <c r="D164" s="9"/>
@@ -5081,7 +5239,7 @@
       <c r="L164" s="9"/>
       <c r="M164" s="11"/>
     </row>
-    <row r="165" spans="2:13" ht="17.25" customHeight="1">
+    <row r="165" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="81"/>
       <c r="C165" s="9"/>
       <c r="D165" s="9"/>
@@ -5095,7 +5253,7 @@
       <c r="L165" s="9"/>
       <c r="M165" s="11"/>
     </row>
-    <row r="166" spans="2:13" ht="18" customHeight="1">
+    <row r="166" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
       <c r="D166" s="9"/>
@@ -5109,7 +5267,7 @@
       <c r="L166" s="9"/>
       <c r="M166" s="11"/>
     </row>
-    <row r="167" spans="2:13">
+    <row r="167" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
       <c r="D167" s="9"/>
@@ -5125,7 +5283,7 @@
       <c r="L167" s="9"/>
       <c r="M167" s="11"/>
     </row>
-    <row r="168" spans="2:13">
+    <row r="168" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
       <c r="D168" s="9"/>
@@ -5139,7 +5297,7 @@
       <c r="L168" s="9"/>
       <c r="M168" s="11"/>
     </row>
-    <row r="169" spans="2:13">
+    <row r="169" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B169" s="23"/>
       <c r="C169" s="23"/>
       <c r="D169" s="23"/>
@@ -5155,12 +5313,12 @@
       <c r="L169" s="9"/>
       <c r="M169" s="11"/>
     </row>
-    <row r="170" spans="2:13" ht="18" customHeight="1">
+    <row r="170" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K170" s="11"/>
       <c r="L170" s="11"/>
       <c r="M170" s="11"/>
     </row>
-    <row r="171" spans="2:13">
+    <row r="171" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C171" s="69" t="s">
         <v>112</v>
       </c>
@@ -5170,7 +5328,7 @@
       <c r="L171" s="11"/>
       <c r="M171" s="11"/>
     </row>
-    <row r="172" spans="2:13">
+    <row r="172" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B172" s="76" t="s">
         <v>113</v>
       </c>
@@ -5186,7 +5344,7 @@
       <c r="L172" s="11"/>
       <c r="M172" s="11"/>
     </row>
-    <row r="173" spans="2:13">
+    <row r="173" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>114</v>
       </c>
@@ -5196,7 +5354,7 @@
       <c r="L173" s="11"/>
       <c r="M173" s="11"/>
     </row>
-    <row r="174" spans="2:13" ht="25.8">
+    <row r="174" spans="2:13" ht="25.8" x14ac:dyDescent="0.4">
       <c r="B174" t="s">
         <v>97</v>
       </c>
@@ -5205,46 +5363,46 @@
       <c r="K174" s="86"/>
       <c r="L174" s="86"/>
     </row>
-    <row r="175" spans="2:13">
+    <row r="175" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="176" spans="2:13">
+    <row r="176" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="177" spans="2:13">
+    <row r="177" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="178" spans="2:13">
+    <row r="178" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="181" spans="2:13" ht="22.2">
+    <row r="181" spans="2:13" ht="22.2" x14ac:dyDescent="0.3">
       <c r="L181" s="87"/>
       <c r="M181" s="65"/>
     </row>
-    <row r="200" ht="18" customHeight="1"/>
-    <row r="215" spans="12:15" ht="22.2">
+    <row r="200" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="12:15" ht="22.2" x14ac:dyDescent="0.3">
       <c r="L215" s="90"/>
       <c r="M215" s="90"/>
     </row>
-    <row r="217" spans="12:15">
+    <row r="217" spans="12:15" x14ac:dyDescent="0.25">
       <c r="O217" s="84"/>
     </row>
-    <row r="226" spans="2:14">
+    <row r="226" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F226" s="76"/>
       <c r="G226" s="76"/>
       <c r="H226" s="76"/>
       <c r="I226" s="76"/>
       <c r="J226" s="76"/>
     </row>
-    <row r="230" spans="2:14" ht="20.399999999999999">
+    <row r="230" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="H230" s="88"/>
       <c r="I230" s="76"/>
       <c r="J230" s="76"/>
@@ -5253,7 +5411,7 @@
       <c r="M230" s="76"/>
       <c r="N230" s="23"/>
     </row>
-    <row r="235" spans="2:14" ht="25.8">
+    <row r="235" spans="2:14" ht="25.8" x14ac:dyDescent="0.4">
       <c r="B235" s="89"/>
       <c r="C235" s="89"/>
       <c r="D235" s="89"/>
@@ -5261,13 +5419,13 @@
       <c r="F235" s="89"/>
       <c r="G235" s="89"/>
     </row>
-    <row r="330" spans="8:11">
+    <row r="330" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H330" s="76"/>
       <c r="I330" s="76"/>
       <c r="J330" s="76"/>
       <c r="K330" s="76"/>
     </row>
-    <row r="351" spans="2:15" ht="16.2">
+    <row r="351" spans="2:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B351" s="91"/>
       <c r="C351" s="91"/>
       <c r="D351" s="91"/>
@@ -5285,12 +5443,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I139:L139"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="I136:L136"/>
     <mergeCell ref="I137:L137"/>
     <mergeCell ref="I138:L138"/>
-    <mergeCell ref="I139:L139"/>
   </mergeCells>
   <phoneticPr fontId="39" type="noConversion"/>
   <pageMargins left="0.75" right="0.11999999999999998" top="0.17" bottom="0.11999999999999998" header="0.5" footer="0.33"/>
@@ -5305,12 +5463,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="39" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5319,12 +5477,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="39" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>